<commit_message>
FRNFR and Data Dictionary
FRNFR finalized, Data Dictionary near complete (if not complete)
</commit_message>
<xml_diff>
--- a/PD1/PD1 - Data Dictionary1.xlsx
+++ b/PD1/PD1 - Data Dictionary1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyezack\CS445\CS445-Group-Project-\PD1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3F881C6-D419-4718-BB89-83A2910E8115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D2D38F-7D0E-4ABF-B234-E374582E1F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C986EE63-EBB2-4DD3-8339-855DFC45247A}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,12 +36,186 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>COLUMN NAME</t>
+  </si>
+  <si>
+    <t>FORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>The unique zip code / postal code of the given city taken as a user input</t>
+  </si>
+  <si>
+    <t>location_name</t>
+  </si>
+  <si>
+    <t>varchar(189)</t>
+  </si>
+  <si>
+    <t>The name of the location specified by ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country_code </t>
+  </si>
+  <si>
+    <t>varchar(2)</t>
+  </si>
+  <si>
+    <t>Two letter ISO 3166-1 alpha-2 code to specify the location's country</t>
+  </si>
+  <si>
+    <t>time_zone</t>
+  </si>
+  <si>
+    <t>varchar(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The time zone which the location belongs to </t>
+  </si>
+  <si>
+    <t>weather_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique ID for the weather entry being displayed </t>
+  </si>
+  <si>
+    <t>weather_date</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>Date of the specified weather entry</t>
+  </si>
+  <si>
+    <t>weather_desc</t>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A summary of the weather for the specified location </t>
+  </si>
+  <si>
+    <t>temperature_current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The current temperature of the specified location </t>
+  </si>
+  <si>
+    <t>temperature_high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMBER </t>
+  </si>
+  <si>
+    <t>The (probable) highest temperature of the day</t>
+  </si>
+  <si>
+    <t>temperature_low</t>
+  </si>
+  <si>
+    <t>humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The humidity percentage for the specified location </t>
+  </si>
+  <si>
+    <t>wind_speed</t>
+  </si>
+  <si>
+    <t>The speed of the wind, given in Miles Per Hour</t>
+  </si>
+  <si>
+    <t>wind_direction</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>The direction that wind is blowing</t>
+  </si>
+  <si>
+    <t>real_feel</t>
+  </si>
+  <si>
+    <t>The calculated "real feel" of the temperature, which considers humidity and wind</t>
+  </si>
+  <si>
+    <t>clothing_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">references the current temperature and chooses a corresponding clothing item </t>
+  </si>
+  <si>
+    <t xml:space="preserve">clothing_description </t>
+  </si>
+  <si>
+    <t>gives a brief description of what clothing the user should wear for the given temperature</t>
+  </si>
+  <si>
+    <t>clothing_drawing</t>
+  </si>
+  <si>
+    <t>IMAGE</t>
+  </si>
+  <si>
+    <t>an illustration of the recommended clothing items</t>
+  </si>
+  <si>
+    <t>notification_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a unique numerical ID that specifies the type of notification being displayed </t>
+  </si>
+  <si>
+    <t>notification_type</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a written term displayed to the user that corresponds to the given ID number </t>
+  </si>
+  <si>
+    <t>notification_content</t>
+  </si>
+  <si>
+    <t>varchar(40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a description of the notification being displayed </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,8 +241,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,17 +564,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048BCD27-5C23-41BD-9D09-F42D56100E1F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="79.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8FD2FACC2314549B73824173580303D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f24e73478bcad6d109eebd3c912e8837">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2e0f097d-079e-4fb3-8506-ecdfbcdbb5cf" xmlns:ns4="a11b3c9f-580f-4c00-b756-074412dd809e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df8a4258ac4fb70b9408712c601943aa" ns3:_="" ns4:_="">
     <xsd:import namespace="2e0f097d-079e-4fb3-8506-ecdfbcdbb5cf"/>
@@ -627,36 +1270,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFA0AAA9-5E6F-4B9D-A62D-6FF417D7D4B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB720773-6739-43DF-BBC7-7B92E06D17A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2e0f097d-079e-4fb3-8506-ecdfbcdbb5cf"/>
-    <ds:schemaRef ds:uri="a11b3c9f-580f-4c00-b756-074412dd809e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -679,9 +1296,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB720773-6739-43DF-BBC7-7B92E06D17A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFA0AAA9-5E6F-4B9D-A62D-6FF417D7D4B5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2e0f097d-079e-4fb3-8506-ecdfbcdbb5cf"/>
+    <ds:schemaRef ds:uri="a11b3c9f-580f-4c00-b756-074412dd809e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>